<commit_message>
used insert many to reduce query fire
</commit_message>
<xml_diff>
--- a/Excel/test2.xlsx
+++ b/Excel/test2.xlsx
@@ -64,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,82 +398,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
         <v>userName</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>email</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>password</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>role</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
+        <v>_id</v>
+      </c>
+      <c r="G1" t="str">
+        <v>date</v>
+      </c>
+      <c r="H1" t="str">
+        <v>__v</v>
+      </c>
+      <c r="I1" t="str">
         <v>err</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>ov5egjxyvn6ytttmhtlt</v>
+      </c>
+      <c r="B2" t="str">
         <v>test_1</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <v>test_1@gmail.com</v>
       </c>
-      <c r="C2" t="str">
-        <v>5WOvk6XA</v>
-      </c>
       <c r="D2" t="str">
+        <v>VW5OGxrS</v>
+      </c>
+      <c r="E2" t="str">
         <v>user</v>
       </c>
-      <c r="E2" t="str">
-        <v>user already exist</v>
+      <c r="G2" s="1">
+        <v>44963.47878810185</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="str">
+        <v>E11000 duplicate key error collection: test.users index: userName_1 dup key: { userName: "test_1" }</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>dqu7x73wxhtc3fhfllpl</v>
+      </c>
+      <c r="B3" t="str">
         <v>test_2</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
         <v>test_2@gamil.com</v>
       </c>
-      <c r="C3" t="str">
-        <v>k7Lep81L</v>
-      </c>
       <c r="D3" t="str">
+        <v>wlxva8wJ</v>
+      </c>
+      <c r="E3" t="str">
         <v>user</v>
       </c>
-      <c r="E3" t="str">
-        <v>user already exist</v>
+      <c r="G3" s="1">
+        <v>44963.478788113425</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="str">
+        <v>E11000 duplicate key error collection: test.users index: userName_1 dup key: { userName: "test_2" }</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
+        <v>w8503zm8pmpa3fv0j6p0</v>
+      </c>
+      <c r="B4" t="str">
         <v>test_3</v>
       </c>
-      <c r="B4" t="str">
+      <c r="C4" t="str">
         <v>test_3@gmail.com</v>
       </c>
-      <c r="C4" t="str">
-        <v>XUsCJ1Ay</v>
-      </c>
       <c r="D4" t="str">
-        <v>user</v>
+        <v>PfzwR9JA</v>
       </c>
       <c r="E4" t="str">
-        <v>user already exist</v>
+        <v>vendor</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44963.478788113425</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="str">
+        <v>E11000 duplicate key error collection: test.users index: userName_1 dup key: { userName: "test_3" }</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>